<commit_message>
Updating weight measurements and adding new food log files
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>FoodID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -54,19 +51,44 @@
   </si>
   <si>
     <t>WaterTargetAchieved</t>
+  </si>
+  <si>
+    <t>01-01-2018</t>
+  </si>
+  <si>
+    <t>02-01-2018</t>
+  </si>
+  <si>
+    <t>03-01-2018</t>
+  </si>
+  <si>
+    <t>04-01-2018</t>
+  </si>
+  <si>
+    <t>05-01-2018</t>
+  </si>
+  <si>
+    <t>06-01-2018</t>
+  </si>
+  <si>
+    <t>07-01-2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,14 +108,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,57 +432,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.7265625" style="3"/>
+    <col min="6" max="6" width="11.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J2" t="str">
-        <f>IF(I2&gt;2500,"Yes","No")</f>
+      <c r="B2" s="3">
+        <v>1221</v>
+      </c>
+      <c r="C2" s="3">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <v>614</v>
+      </c>
+      <c r="G2" s="3">
+        <v>150</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2250</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(H2&gt;2200,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1156</v>
+      </c>
+      <c r="C3" s="3">
+        <v>48</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>128</v>
+      </c>
+      <c r="F3" s="3">
+        <v>847</v>
+      </c>
+      <c r="G3" s="3">
+        <v>48</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2250</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I8" si="0">IF(H3&gt;2200,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1861</v>
+      </c>
+      <c r="C4" s="3">
+        <v>33</v>
+      </c>
+      <c r="D4" s="3">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <v>252</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1604</v>
+      </c>
+      <c r="G4" s="3">
+        <v>82</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
         <v>No</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1831</v>
+      </c>
+      <c r="C5" s="3">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3">
+        <v>222</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3423</v>
+      </c>
+      <c r="G5" s="3">
+        <v>61</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1250</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1227</v>
+      </c>
+      <c r="C6" s="3">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>140</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1348</v>
+      </c>
+      <c r="G6" s="3">
+        <v>71</v>
+      </c>
+      <c r="H6" s="3">
+        <v>3000</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1597</v>
+      </c>
+      <c r="C7" s="3">
+        <v>48</v>
+      </c>
+      <c r="D7" s="3">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3">
+        <v>127</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1933</v>
+      </c>
+      <c r="G7" s="3">
+        <v>167</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2800</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1410</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3">
+        <v>106</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1081</v>
+      </c>
+      <c r="G8" s="3">
+        <v>146</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2300</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating weight measurements and food log files
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,30 @@
   </si>
   <si>
     <t>07-01-2018</t>
+  </si>
+  <si>
+    <t>WeekID</t>
+  </si>
+  <si>
+    <t>08-01-2018</t>
+  </si>
+  <si>
+    <t>09-01-2018</t>
+  </si>
+  <si>
+    <t>10-01-2018</t>
+  </si>
+  <si>
+    <t>11-01-2018</t>
+  </si>
+  <si>
+    <t>12-01-2018</t>
+  </si>
+  <si>
+    <t>13-01-2018</t>
+  </si>
+  <si>
+    <t>14-01-2018</t>
   </si>
 </sst>
 </file>
@@ -112,11 +136,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,244 +471,500 @@
     <col min="6" max="6" width="11.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
         <v>1221</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>18</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>12</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>100</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>614</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>150</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>2250</v>
       </c>
-      <c r="I2" t="str">
-        <f>IF(H2&gt;2200,"Yes","No")</f>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" t="str">
+        <f>IF(I2&gt;2200,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
         <v>1156</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>48</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>10</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>128</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>847</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>48</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>2250</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I8" si="0">IF(H3&gt;2200,"Yes","No")</f>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J15" si="0">IF(I3&gt;2200,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
         <v>1861</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>33</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>16</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>252</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>1604</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>82</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>1000</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
         <v>1831</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>33</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>11</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>222</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>3423</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>61</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>1250</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
         <v>1227</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>35</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>140</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>1348</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>71</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>3000</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
         <v>1597</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>48</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>16</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>127</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>1933</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>167</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>2800</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
         <v>1410</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>44</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>16</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>106</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>1081</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>146</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>2300</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1469</v>
+      </c>
+      <c r="D9" s="3">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3">
+        <v>131</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3790</v>
+      </c>
+      <c r="H9" s="3">
+        <v>137</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2300</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1497</v>
+      </c>
+      <c r="D10" s="3">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3">
+        <v>15</v>
+      </c>
+      <c r="F10" s="3">
+        <v>143</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1385</v>
+      </c>
+      <c r="H10" s="3">
+        <v>159</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2550</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1698</v>
+      </c>
+      <c r="D11" s="3">
+        <v>49</v>
+      </c>
+      <c r="E11" s="3">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3">
+        <v>150</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1803</v>
+      </c>
+      <c r="H11" s="3">
+        <v>159</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2550</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1588</v>
+      </c>
+      <c r="D12" s="3">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3">
+        <v>27</v>
+      </c>
+      <c r="F12" s="3">
+        <v>173</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1601</v>
+      </c>
+      <c r="H12" s="3">
+        <v>142</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2300</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1605</v>
+      </c>
+      <c r="D13" s="3">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3">
+        <v>135</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1747</v>
+      </c>
+      <c r="H13" s="3">
+        <v>153</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1516</v>
+      </c>
+      <c r="D14" s="3">
+        <v>33</v>
+      </c>
+      <c r="E14" s="3">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3">
+        <v>171</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1163</v>
+      </c>
+      <c r="H14" s="3">
+        <v>129</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1545</v>
+      </c>
+      <c r="D15" s="3">
+        <v>76</v>
+      </c>
+      <c r="E15" s="3">
+        <v>14</v>
+      </c>
+      <c r="F15" s="3">
+        <v>76</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2680</v>
+      </c>
+      <c r="H15" s="3">
+        <v>135</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2350</v>
+      </c>
+      <c r="J15" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>

</xml_diff>

<commit_message>
Updating weight measurements and updating foodlogs 22/01/2018
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +99,27 @@
   </si>
   <si>
     <t>14-01-2018</t>
+  </si>
+  <si>
+    <t>15-01-2018</t>
+  </si>
+  <si>
+    <t>16-01-2018</t>
+  </si>
+  <si>
+    <t>17-01-2018</t>
+  </si>
+  <si>
+    <t>18-01-2018</t>
+  </si>
+  <si>
+    <t>19-01-2018</t>
+  </si>
+  <si>
+    <t>20-01-2018</t>
+  </si>
+  <si>
+    <t>21-01-2018</t>
   </si>
 </sst>
 </file>
@@ -158,6 +182,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Foods"/>
+      <sheetName val="Food Log 20180115"/>
+      <sheetName val="Food Log 20180116"/>
+      <sheetName val="Food Log 20180117"/>
+      <sheetName val="Food Log 20180118"/>
+      <sheetName val="Food Log 20180119"/>
+      <sheetName val="Food Log 20180120"/>
+      <sheetName val="Food Log 20180121"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,7 +620,7 @@
         <v>2250</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J15" si="0">IF(I3&gt;2200,"Yes","No")</f>
+        <f t="shared" ref="J3:J22" si="0">IF(I3&gt;2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -969,7 +1020,239 @@
         <v>Yes</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1523</v>
+      </c>
+      <c r="D16" s="3">
+        <v>39</v>
+      </c>
+      <c r="E16" s="3">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3">
+        <v>180</v>
+      </c>
+      <c r="G16" s="3">
+        <v>888</v>
+      </c>
+      <c r="H16" s="3">
+        <v>109</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2600</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1799</v>
+      </c>
+      <c r="D17" s="3">
+        <v>39</v>
+      </c>
+      <c r="E17" s="3">
+        <v>25</v>
+      </c>
+      <c r="F17" s="3">
+        <v>192</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3127</v>
+      </c>
+      <c r="H17" s="3">
+        <v>172</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1704</v>
+      </c>
+      <c r="D18" s="3">
+        <v>40</v>
+      </c>
+      <c r="E18" s="3">
+        <v>40</v>
+      </c>
+      <c r="F18" s="3">
+        <v>164</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1683</v>
+      </c>
+      <c r="H18" s="3">
+        <v>175</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2350</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1969</v>
+      </c>
+      <c r="D19" s="3">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3">
+        <v>20</v>
+      </c>
+      <c r="F19" s="3">
+        <v>185</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2380</v>
+      </c>
+      <c r="H19" s="3">
+        <v>196</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1561</v>
+      </c>
+      <c r="D20" s="3">
+        <v>49</v>
+      </c>
+      <c r="E20" s="3">
+        <v>30</v>
+      </c>
+      <c r="F20" s="3">
+        <v>118</v>
+      </c>
+      <c r="G20" s="3">
+        <v>6872</v>
+      </c>
+      <c r="H20" s="3">
+        <v>146</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2300</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1350</v>
+      </c>
+      <c r="D21" s="3">
+        <v>39</v>
+      </c>
+      <c r="E21" s="3">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3">
+        <v>102</v>
+      </c>
+      <c r="G21" s="3">
+        <v>4947</v>
+      </c>
+      <c r="H21" s="3">
+        <v>135</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1613</v>
+      </c>
+      <c r="D22" s="3">
+        <v>58</v>
+      </c>
+      <c r="E22" s="3">
+        <v>24</v>
+      </c>
+      <c r="F22" s="3">
+        <v>131</v>
+      </c>
+      <c r="G22" s="3">
+        <v>4088</v>
+      </c>
+      <c r="H22" s="3">
+        <v>142</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2300</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding updated FoodLog and WeightMeasurements
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +117,30 @@
   </si>
   <si>
     <t>21-01-2018</t>
+  </si>
+  <si>
+    <t>22-01-2018</t>
+  </si>
+  <si>
+    <t>23-01-2018</t>
+  </si>
+  <si>
+    <t>24-01-2018</t>
+  </si>
+  <si>
+    <t>25-01-2018</t>
+  </si>
+  <si>
+    <t>26-01-2018</t>
+  </si>
+  <si>
+    <t>27-01-2018</t>
+  </si>
+  <si>
+    <t>28-01-2018</t>
+  </si>
+  <si>
+    <t>30-01-2018</t>
   </si>
 </sst>
 </file>
@@ -160,12 +181,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,33 +205,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Foods"/>
-      <sheetName val="Food Log 20180115"/>
-      <sheetName val="Food Log 20180116"/>
-      <sheetName val="Food Log 20180117"/>
-      <sheetName val="Food Log 20180118"/>
-      <sheetName val="Food Log 20180119"/>
-      <sheetName val="Food Log 20180120"/>
-      <sheetName val="Food Log 20180121"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -508,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,7 +616,7 @@
         <v>2250</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J22" si="0">IF(I3&gt;2200,"Yes","No")</f>
+        <f t="shared" ref="J3:J30" si="0">IF(I3&gt;2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -1247,6 +1243,270 @@
         <v>2300</v>
       </c>
       <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="3">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1719</v>
+      </c>
+      <c r="D23" s="3">
+        <v>58</v>
+      </c>
+      <c r="E23" s="3">
+        <v>22</v>
+      </c>
+      <c r="F23" s="3">
+        <v>123</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4747</v>
+      </c>
+      <c r="H23" s="3">
+        <v>176</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2200</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1976</v>
+      </c>
+      <c r="D24" s="3">
+        <v>66</v>
+      </c>
+      <c r="E24" s="3">
+        <v>23</v>
+      </c>
+      <c r="F24" s="3">
+        <v>257</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4536</v>
+      </c>
+      <c r="H24" s="3">
+        <v>95</v>
+      </c>
+      <c r="I24" s="3">
+        <v>5500</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="3">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6">
+        <v>674</v>
+      </c>
+      <c r="D25" s="3">
+        <v>17</v>
+      </c>
+      <c r="E25" s="3">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3">
+        <v>67</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2042</v>
+      </c>
+      <c r="H25" s="3">
+        <v>55</v>
+      </c>
+      <c r="I25" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="3">
+        <v>4</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1193</v>
+      </c>
+      <c r="D26" s="3">
+        <v>44</v>
+      </c>
+      <c r="E26" s="3">
+        <v>19</v>
+      </c>
+      <c r="F26" s="3">
+        <v>101</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3496</v>
+      </c>
+      <c r="H26" s="3">
+        <v>88</v>
+      </c>
+      <c r="I26" s="3">
+        <v>2000</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3">
+        <v>4</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1622</v>
+      </c>
+      <c r="D27" s="3">
+        <v>26</v>
+      </c>
+      <c r="E27" s="3">
+        <v>31</v>
+      </c>
+      <c r="F27" s="3">
+        <v>197</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1026</v>
+      </c>
+      <c r="H27" s="3">
+        <v>134</v>
+      </c>
+      <c r="I27" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1691</v>
+      </c>
+      <c r="D28" s="3">
+        <v>48</v>
+      </c>
+      <c r="E28" s="3">
+        <v>35</v>
+      </c>
+      <c r="F28" s="3">
+        <v>220</v>
+      </c>
+      <c r="G28" s="3">
+        <v>3663</v>
+      </c>
+      <c r="H28" s="3">
+        <v>95</v>
+      </c>
+      <c r="I28" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="3">
+        <v>4</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1181</v>
+      </c>
+      <c r="D29" s="3">
+        <v>59</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3">
+        <v>76</v>
+      </c>
+      <c r="G29" s="3">
+        <v>4727</v>
+      </c>
+      <c r="H29" s="3">
+        <v>81</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1500</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="3">
+        <v>5</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1302</v>
+      </c>
+      <c r="D30" s="3">
+        <v>37</v>
+      </c>
+      <c r="E30" s="3">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3">
+        <v>158</v>
+      </c>
+      <c r="G30" s="3">
+        <v>3567</v>
+      </c>
+      <c r="H30" s="3">
+        <v>69</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>

</xml_diff>

<commit_message>
Adding updated FoodLog 11/02/2018
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,42 @@
   </si>
   <si>
     <t>30-01-2018</t>
+  </si>
+  <si>
+    <t>31-01-2018</t>
+  </si>
+  <si>
+    <t>01-02-2018</t>
+  </si>
+  <si>
+    <t>02-02-2018</t>
+  </si>
+  <si>
+    <t>03-02-2018</t>
+  </si>
+  <si>
+    <t>04-02-2018</t>
+  </si>
+  <si>
+    <t>05-02-2018</t>
+  </si>
+  <si>
+    <t>06-02-2018</t>
+  </si>
+  <si>
+    <t>07-02-2018</t>
+  </si>
+  <si>
+    <t>08-02-2018</t>
+  </si>
+  <si>
+    <t>09-02-2018</t>
+  </si>
+  <si>
+    <t>10-02-2018</t>
+  </si>
+  <si>
+    <t>11-02-2018</t>
   </si>
 </sst>
 </file>
@@ -181,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -189,6 +225,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +620,7 @@
         <v>2250</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(I2&gt;2200,"Yes","No")</f>
+        <f>IF(I2&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -616,7 +653,7 @@
         <v>2250</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J30" si="0">IF(I3&gt;2200,"Yes","No")</f>
+        <f t="shared" ref="J3:J42" si="0">IF(I3&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -1277,7 +1314,7 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -1507,6 +1544,402 @@
         <v>2250</v>
       </c>
       <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>5</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1693</v>
+      </c>
+      <c r="D31" s="3">
+        <v>70</v>
+      </c>
+      <c r="E31" s="3">
+        <v>15</v>
+      </c>
+      <c r="F31" s="3">
+        <v>106</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2710</v>
+      </c>
+      <c r="H31" s="3">
+        <v>162</v>
+      </c>
+      <c r="I31" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="3">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1700</v>
+      </c>
+      <c r="D32" s="3">
+        <v>67</v>
+      </c>
+      <c r="E32" s="3">
+        <v>26</v>
+      </c>
+      <c r="F32" s="3">
+        <v>140</v>
+      </c>
+      <c r="G32" s="3">
+        <v>2723</v>
+      </c>
+      <c r="H32" s="3">
+        <v>136</v>
+      </c>
+      <c r="I32" s="3">
+        <v>2200</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="3">
+        <v>5</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1491</v>
+      </c>
+      <c r="D33" s="3">
+        <v>59</v>
+      </c>
+      <c r="E33" s="3">
+        <v>22</v>
+      </c>
+      <c r="F33" s="3">
+        <v>109</v>
+      </c>
+      <c r="G33" s="3">
+        <v>2866</v>
+      </c>
+      <c r="H33" s="3">
+        <v>128</v>
+      </c>
+      <c r="I33" s="3">
+        <v>2200</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="3">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1454</v>
+      </c>
+      <c r="D34" s="3">
+        <v>56</v>
+      </c>
+      <c r="E34" s="3">
+        <v>27</v>
+      </c>
+      <c r="F34" s="3">
+        <v>110</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2279</v>
+      </c>
+      <c r="H34" s="3">
+        <v>124</v>
+      </c>
+      <c r="I34" s="3">
+        <v>2450</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1384</v>
+      </c>
+      <c r="D35" s="3">
+        <v>26</v>
+      </c>
+      <c r="E35" s="3">
+        <v>34</v>
+      </c>
+      <c r="F35" s="3">
+        <v>192</v>
+      </c>
+      <c r="G35" s="3">
+        <v>2258</v>
+      </c>
+      <c r="H35" s="3">
+        <v>101</v>
+      </c>
+      <c r="I35" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="3">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1308</v>
+      </c>
+      <c r="D36" s="3">
+        <v>53</v>
+      </c>
+      <c r="E36" s="3">
+        <v>18</v>
+      </c>
+      <c r="F36" s="3">
+        <v>97</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1896</v>
+      </c>
+      <c r="H36" s="3">
+        <v>116</v>
+      </c>
+      <c r="I36" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="3">
+        <v>6</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2730</v>
+      </c>
+      <c r="D37" s="3">
+        <v>85</v>
+      </c>
+      <c r="E37" s="3">
+        <v>27</v>
+      </c>
+      <c r="F37" s="3">
+        <v>340</v>
+      </c>
+      <c r="G37" s="3">
+        <v>4250</v>
+      </c>
+      <c r="H37" s="3">
+        <v>129</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1000</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="3">
+        <v>6</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1643</v>
+      </c>
+      <c r="D38" s="3">
+        <v>35</v>
+      </c>
+      <c r="E38" s="3">
+        <v>22</v>
+      </c>
+      <c r="F38" s="3">
+        <v>153</v>
+      </c>
+      <c r="G38" s="3">
+        <v>2490</v>
+      </c>
+      <c r="H38" s="3">
+        <v>163</v>
+      </c>
+      <c r="I38" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="3">
+        <v>6</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1840</v>
+      </c>
+      <c r="D39" s="3">
+        <v>60</v>
+      </c>
+      <c r="E39" s="3">
+        <v>25</v>
+      </c>
+      <c r="F39" s="3">
+        <v>132</v>
+      </c>
+      <c r="G39" s="3">
+        <v>2982</v>
+      </c>
+      <c r="H39" s="3">
+        <v>184</v>
+      </c>
+      <c r="I39" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="3">
+        <v>6</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1704</v>
+      </c>
+      <c r="D40" s="3">
+        <v>40</v>
+      </c>
+      <c r="E40" s="3">
+        <v>32</v>
+      </c>
+      <c r="F40" s="3">
+        <v>184</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1885</v>
+      </c>
+      <c r="H40" s="3">
+        <v>148</v>
+      </c>
+      <c r="I40" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="3">
+        <v>6</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1527</v>
+      </c>
+      <c r="D41" s="3">
+        <v>37</v>
+      </c>
+      <c r="E41" s="3">
+        <v>20</v>
+      </c>
+      <c r="F41" s="3">
+        <v>138</v>
+      </c>
+      <c r="G41" s="3">
+        <v>2697</v>
+      </c>
+      <c r="H41" s="3">
+        <v>133</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="3">
+        <v>6</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1476</v>
+      </c>
+      <c r="D42" s="3">
+        <v>38</v>
+      </c>
+      <c r="E42" s="3">
+        <v>13</v>
+      </c>
+      <c r="F42" s="3">
+        <v>101</v>
+      </c>
+      <c r="G42" s="3">
+        <v>2152</v>
+      </c>
+      <c r="H42" s="3">
+        <v>164</v>
+      </c>
+      <c r="I42" s="3">
+        <v>2250</v>
+      </c>
+      <c r="J42" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>

</xml_diff>

<commit_message>
Updating FoodLog 25/03/2018 and README.md file
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D486EC02-93A5-43D7-B5A2-C676D9584EE4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08B9A83-7308-4219-A5B3-BE62779D108C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{2FDD2F76-DCBF-453F-AE6A-59BCC3816064}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -280,6 +280,30 @@
   </si>
   <si>
     <t>17-03-2018</t>
+  </si>
+  <si>
+    <t>18-03-2018</t>
+  </si>
+  <si>
+    <t>19-03-2018</t>
+  </si>
+  <si>
+    <t>20-03-2018</t>
+  </si>
+  <si>
+    <t>21-03-2018</t>
+  </si>
+  <si>
+    <t>22-03-2018</t>
+  </si>
+  <si>
+    <t>23-03-2018</t>
+  </si>
+  <si>
+    <t>24-03-2018</t>
+  </si>
+  <si>
+    <t>UnderEaten</t>
   </si>
 </sst>
 </file>
@@ -331,7 +355,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -345,6 +369,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -661,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,9 +703,10 @@
     <col min="8" max="8" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,8 +737,12 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -744,8 +774,12 @@
         <f>IF(I2&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" t="str">
+        <f>IF(C2&lt;=1800,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -774,11 +808,15 @@
         <v>2250</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J76" si="0">IF(I3&gt;=2200,"Yes","No")</f>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" ref="J3:J83" si="0">IF(I3&gt;=2200,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="1">IF(C3&lt;=1800,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -810,8 +848,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -843,8 +885,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -876,8 +922,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -909,8 +959,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -942,8 +996,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -975,8 +1033,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1008,8 +1070,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1041,8 +1107,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1074,8 +1144,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1107,8 +1181,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1140,8 +1218,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
@@ -1173,8 +1255,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1206,8 +1292,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1239,8 +1329,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1272,8 +1366,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1305,8 +1403,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1338,8 +1440,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1371,8 +1477,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1404,8 +1514,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
@@ -1437,8 +1551,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>32</v>
       </c>
@@ -1470,8 +1588,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>33</v>
       </c>
@@ -1503,8 +1625,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>34</v>
       </c>
@@ -1536,8 +1662,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>35</v>
       </c>
@@ -1569,8 +1699,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>36</v>
       </c>
@@ -1602,8 +1736,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>37</v>
       </c>
@@ -1635,8 +1773,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>38</v>
       </c>
@@ -1668,8 +1810,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>39</v>
       </c>
@@ -1701,8 +1847,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>40</v>
       </c>
@@ -1734,8 +1884,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>41</v>
       </c>
@@ -1767,8 +1921,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>42</v>
       </c>
@@ -1800,8 +1958,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>43</v>
       </c>
@@ -1833,8 +1995,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>44</v>
       </c>
@@ -1866,8 +2032,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>45</v>
       </c>
@@ -1899,8 +2069,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>46</v>
       </c>
@@ -1932,8 +2106,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>47</v>
       </c>
@@ -1965,8 +2143,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>48</v>
       </c>
@@ -1998,8 +2180,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>49</v>
       </c>
@@ -2031,8 +2217,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>50</v>
       </c>
@@ -2064,8 +2254,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>51</v>
       </c>
@@ -2097,8 +2291,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>52</v>
       </c>
@@ -2130,8 +2328,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>53</v>
       </c>
@@ -2163,8 +2365,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K45" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>54</v>
       </c>
@@ -2196,8 +2402,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K46" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>55</v>
       </c>
@@ -2229,8 +2439,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K47" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>56</v>
       </c>
@@ -2262,8 +2476,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K48" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>57</v>
       </c>
@@ -2295,8 +2513,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K49" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>58</v>
       </c>
@@ -2328,8 +2550,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K50" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>59</v>
       </c>
@@ -2361,8 +2587,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K51" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>60</v>
       </c>
@@ -2394,8 +2624,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K52" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>61</v>
       </c>
@@ -2427,8 +2661,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K53" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>62</v>
       </c>
@@ -2460,8 +2698,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K54" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>63</v>
       </c>
@@ -2493,8 +2735,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K55" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>64</v>
       </c>
@@ -2526,8 +2772,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K56" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>65</v>
       </c>
@@ -2559,8 +2809,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K57" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>66</v>
       </c>
@@ -2592,8 +2846,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K58" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>67</v>
       </c>
@@ -2625,8 +2883,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K59" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>68</v>
       </c>
@@ -2658,8 +2920,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K60" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>69</v>
       </c>
@@ -2691,8 +2957,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K61" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>70</v>
       </c>
@@ -2724,8 +2994,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K62" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>71</v>
       </c>
@@ -2757,8 +3031,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K63" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>72</v>
       </c>
@@ -2790,8 +3068,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K64" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>73</v>
       </c>
@@ -2823,8 +3105,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K65" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>74</v>
       </c>
@@ -2856,8 +3142,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K66" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>75</v>
       </c>
@@ -2889,8 +3179,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K83" si="2">IF(C67&lt;=1800,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
         <v>76</v>
       </c>
@@ -2922,8 +3216,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K68" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>77</v>
       </c>
@@ -2955,8 +3253,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K69" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>78</v>
       </c>
@@ -2988,8 +3290,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K70" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
         <v>79</v>
       </c>
@@ -3021,8 +3327,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K71" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
         <v>80</v>
       </c>
@@ -3054,8 +3364,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K72" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
         <v>81</v>
       </c>
@@ -3087,8 +3401,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K73" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
         <v>82</v>
       </c>
@@ -3120,8 +3438,12 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K74" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
         <v>83</v>
       </c>
@@ -3153,8 +3475,12 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K75" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
         <v>84</v>
       </c>
@@ -3184,6 +3510,269 @@
       </c>
       <c r="J76" t="str">
         <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A77" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="3">
+        <v>11</v>
+      </c>
+      <c r="C77" s="12">
+        <v>1539</v>
+      </c>
+      <c r="D77" s="3">
+        <v>49</v>
+      </c>
+      <c r="E77" s="3">
+        <v>9</v>
+      </c>
+      <c r="F77" s="3">
+        <v>64</v>
+      </c>
+      <c r="G77" s="3">
+        <v>1315</v>
+      </c>
+      <c r="H77" s="3">
+        <v>182</v>
+      </c>
+      <c r="I77" s="3">
+        <v>3000</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A78" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="3">
+        <v>12</v>
+      </c>
+      <c r="C78" s="12">
+        <v>2200</v>
+      </c>
+      <c r="D78" s="3">
+        <v>67</v>
+      </c>
+      <c r="E78" s="3">
+        <v>27</v>
+      </c>
+      <c r="F78" s="3">
+        <v>149</v>
+      </c>
+      <c r="G78" s="3">
+        <v>2029</v>
+      </c>
+      <c r="H78" s="3">
+        <v>242</v>
+      </c>
+      <c r="I78" s="3">
+        <v>3000</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K78" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A79" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="3">
+        <v>12</v>
+      </c>
+      <c r="C79" s="12">
+        <v>1680</v>
+      </c>
+      <c r="D79" s="3">
+        <v>67</v>
+      </c>
+      <c r="E79" s="3">
+        <v>9</v>
+      </c>
+      <c r="F79" s="3">
+        <v>97</v>
+      </c>
+      <c r="G79" s="3">
+        <v>2060</v>
+      </c>
+      <c r="H79" s="3">
+        <v>163</v>
+      </c>
+      <c r="I79" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K79" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A80" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80" s="3">
+        <v>12</v>
+      </c>
+      <c r="C80" s="12">
+        <v>1554</v>
+      </c>
+      <c r="D80" s="3">
+        <v>65</v>
+      </c>
+      <c r="E80" s="3">
+        <v>5</v>
+      </c>
+      <c r="F80" s="3">
+        <v>99</v>
+      </c>
+      <c r="G80" s="3">
+        <v>1940</v>
+      </c>
+      <c r="H80" s="3">
+        <v>127</v>
+      </c>
+      <c r="I80" s="3">
+        <v>3000</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K80" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A81" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" s="3">
+        <v>12</v>
+      </c>
+      <c r="C81" s="12">
+        <v>1853</v>
+      </c>
+      <c r="D81" s="3">
+        <v>60</v>
+      </c>
+      <c r="E81" s="3">
+        <v>8</v>
+      </c>
+      <c r="F81" s="3">
+        <v>104</v>
+      </c>
+      <c r="G81" s="3">
+        <v>2315</v>
+      </c>
+      <c r="H81" s="3">
+        <v>197</v>
+      </c>
+      <c r="I81" s="3">
+        <v>3000</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K81" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A82" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="3">
+        <v>12</v>
+      </c>
+      <c r="C82" s="12">
+        <v>2145</v>
+      </c>
+      <c r="D82" s="3">
+        <v>65</v>
+      </c>
+      <c r="E82" s="3">
+        <v>11</v>
+      </c>
+      <c r="F82" s="3">
+        <v>209</v>
+      </c>
+      <c r="G82" s="3">
+        <v>4112</v>
+      </c>
+      <c r="H82" s="3">
+        <v>97</v>
+      </c>
+      <c r="I82" s="3">
+        <v>3500</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K82" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A83" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" s="3">
+        <v>12</v>
+      </c>
+      <c r="C83" s="12">
+        <v>1479</v>
+      </c>
+      <c r="D83" s="3">
+        <v>85</v>
+      </c>
+      <c r="E83" s="3">
+        <v>5</v>
+      </c>
+      <c r="F83" s="3">
+        <v>63</v>
+      </c>
+      <c r="G83" s="3">
+        <v>2125</v>
+      </c>
+      <c r="H83" s="3">
+        <v>105</v>
+      </c>
+      <c r="I83" s="3">
+        <v>1000</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="K83" t="str">
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating FoodLog 15/04/2018 file
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6F50AA-15F7-46E4-B402-08B3B0799315}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B82974E-379B-4169-9898-6587B36CAF6E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{2FDD2F76-DCBF-453F-AE6A-59BCC3816064}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -346,6 +346,27 @@
   </si>
   <si>
     <t>08-04-2018</t>
+  </si>
+  <si>
+    <t>09-04-2018</t>
+  </si>
+  <si>
+    <t>10-04-2018</t>
+  </si>
+  <si>
+    <t>11-04-2018</t>
+  </si>
+  <si>
+    <t>12-04-2018</t>
+  </si>
+  <si>
+    <t>13-04-2018</t>
+  </si>
+  <si>
+    <t>14-04-2018</t>
+  </si>
+  <si>
+    <t>15-04-2018</t>
   </si>
 </sst>
 </file>
@@ -397,7 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -411,6 +432,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -730,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J94" sqref="J94"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3018,11 +3040,11 @@
         <v>3250</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I98" si="2">IF(H67&gt;=2200,"Yes","No")</f>
+        <f t="shared" ref="I67:I105" si="2">IF(H67&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J98" si="3">IF(B67&lt;=1800,"Yes","No")</f>
+        <f t="shared" ref="J67:J105" si="3">IF(B67&lt;=1800,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4078,6 +4100,244 @@
       <c r="J98" t="str">
         <f t="shared" si="3"/>
         <v>No</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99" s="6">
+        <v>1256</v>
+      </c>
+      <c r="C99" s="3">
+        <v>63</v>
+      </c>
+      <c r="D99" s="3">
+        <v>2</v>
+      </c>
+      <c r="E99" s="3">
+        <v>101</v>
+      </c>
+      <c r="F99" s="3">
+        <v>2181</v>
+      </c>
+      <c r="G99" s="3">
+        <v>66</v>
+      </c>
+      <c r="H99" s="3">
+        <v>2500</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A100" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" s="6">
+        <v>1299</v>
+      </c>
+      <c r="C100" s="3">
+        <v>31</v>
+      </c>
+      <c r="D100" s="3">
+        <v>8</v>
+      </c>
+      <c r="E100" s="3">
+        <v>134</v>
+      </c>
+      <c r="F100" s="3">
+        <v>1855</v>
+      </c>
+      <c r="G100" s="3">
+        <v>110</v>
+      </c>
+      <c r="H100" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A101" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101" s="6">
+        <v>1545</v>
+      </c>
+      <c r="C101" s="3">
+        <v>62</v>
+      </c>
+      <c r="D101" s="3">
+        <v>9</v>
+      </c>
+      <c r="E101" s="3">
+        <v>10</v>
+      </c>
+      <c r="F101" s="3">
+        <v>2225</v>
+      </c>
+      <c r="G101" s="3">
+        <v>130</v>
+      </c>
+      <c r="H101" s="3">
+        <v>1500</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A102" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" s="6">
+        <v>1548</v>
+      </c>
+      <c r="C102" s="3">
+        <v>54</v>
+      </c>
+      <c r="D102" s="3">
+        <v>3</v>
+      </c>
+      <c r="E102" s="3">
+        <v>117</v>
+      </c>
+      <c r="F102" s="3">
+        <v>2621</v>
+      </c>
+      <c r="G102" s="3">
+        <v>130</v>
+      </c>
+      <c r="H102" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J102" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A103" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103" s="6">
+        <v>1356</v>
+      </c>
+      <c r="C103" s="3">
+        <v>37</v>
+      </c>
+      <c r="D103" s="3">
+        <v>13</v>
+      </c>
+      <c r="E103" s="3">
+        <v>168</v>
+      </c>
+      <c r="F103" s="3">
+        <v>1771</v>
+      </c>
+      <c r="G103" s="3">
+        <v>81</v>
+      </c>
+      <c r="H103" s="3">
+        <v>1750</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J103" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104" s="6">
+        <v>1264</v>
+      </c>
+      <c r="C104" s="3">
+        <v>31</v>
+      </c>
+      <c r="D104" s="3">
+        <v>12</v>
+      </c>
+      <c r="E104" s="3">
+        <v>182</v>
+      </c>
+      <c r="F104" s="3">
+        <v>1709</v>
+      </c>
+      <c r="G104" s="3">
+        <v>55</v>
+      </c>
+      <c r="H104" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I104" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J104" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A105" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" s="6">
+        <v>1209</v>
+      </c>
+      <c r="C105" s="3">
+        <v>31</v>
+      </c>
+      <c r="D105" s="3">
+        <v>16</v>
+      </c>
+      <c r="E105" s="3">
+        <v>166</v>
+      </c>
+      <c r="F105" s="3">
+        <v>1511</v>
+      </c>
+      <c r="G105" s="3">
+        <v>62</v>
+      </c>
+      <c r="H105" s="3">
+        <v>3000</v>
+      </c>
+      <c r="I105" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J105" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating FoodLog files 22/04/2018
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B82974E-379B-4169-9898-6587B36CAF6E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79CD2E6-A5DE-4263-B274-4864BD769BB7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{2FDD2F76-DCBF-453F-AE6A-59BCC3816064}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Date</t>
   </si>
@@ -367,6 +367,24 @@
   </si>
   <si>
     <t>15-04-2018</t>
+  </si>
+  <si>
+    <t>16-04-2018</t>
+  </si>
+  <si>
+    <t>17-04-2018</t>
+  </si>
+  <si>
+    <t>18-04-2018</t>
+  </si>
+  <si>
+    <t>19-04-2018</t>
+  </si>
+  <si>
+    <t>20-04-2018</t>
+  </si>
+  <si>
+    <t>21-04-2018</t>
   </si>
 </sst>
 </file>
@@ -418,7 +436,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -432,6 +450,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -752,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H106" sqref="H106"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="L109" sqref="L109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3040,11 +3059,11 @@
         <v>3250</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I105" si="2">IF(H67&gt;=2200,"Yes","No")</f>
+        <f t="shared" ref="I67:I111" si="2">IF(H67&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J105" si="3">IF(B67&lt;=1800,"Yes","No")</f>
+        <f t="shared" ref="J67:J111" si="3">IF(B67&lt;=1800,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4338,6 +4357,210 @@
       <c r="J105" t="str">
         <f t="shared" si="3"/>
         <v>Yes</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106" s="6">
+        <v>1994</v>
+      </c>
+      <c r="C106" s="3">
+        <v>58</v>
+      </c>
+      <c r="D106" s="3">
+        <v>33</v>
+      </c>
+      <c r="E106" s="3">
+        <v>175</v>
+      </c>
+      <c r="F106" s="3">
+        <v>2468</v>
+      </c>
+      <c r="G106" s="3">
+        <v>177</v>
+      </c>
+      <c r="H106" s="3">
+        <v>3000</v>
+      </c>
+      <c r="I106" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J106" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A107" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B107" s="6">
+        <v>1857</v>
+      </c>
+      <c r="C107" s="3">
+        <v>76</v>
+      </c>
+      <c r="D107" s="3">
+        <v>14</v>
+      </c>
+      <c r="E107" s="3">
+        <v>130</v>
+      </c>
+      <c r="F107" s="3">
+        <v>3506</v>
+      </c>
+      <c r="G107" s="3">
+        <v>155</v>
+      </c>
+      <c r="H107" s="3">
+        <v>3000</v>
+      </c>
+      <c r="I107" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J107" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A108" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B108" s="6">
+        <v>1812</v>
+      </c>
+      <c r="C108" s="3">
+        <v>67</v>
+      </c>
+      <c r="D108" s="3">
+        <v>19</v>
+      </c>
+      <c r="E108" s="3">
+        <v>165</v>
+      </c>
+      <c r="F108" s="3">
+        <v>3077</v>
+      </c>
+      <c r="G108" s="3">
+        <v>127</v>
+      </c>
+      <c r="H108" s="3">
+        <v>3250</v>
+      </c>
+      <c r="I108" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J108" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A109" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B109" s="6">
+        <v>1866</v>
+      </c>
+      <c r="C109" s="3">
+        <v>63</v>
+      </c>
+      <c r="D109" s="3">
+        <v>27</v>
+      </c>
+      <c r="E109" s="3">
+        <v>149</v>
+      </c>
+      <c r="F109" s="3">
+        <v>4621</v>
+      </c>
+      <c r="G109" s="3">
+        <v>171</v>
+      </c>
+      <c r="H109" s="3">
+        <v>2500</v>
+      </c>
+      <c r="I109" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J109" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A110" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" s="6">
+        <v>2607</v>
+      </c>
+      <c r="C110" s="3">
+        <v>103</v>
+      </c>
+      <c r="D110" s="3">
+        <v>17</v>
+      </c>
+      <c r="E110" s="3">
+        <v>277</v>
+      </c>
+      <c r="F110" s="3">
+        <v>4224</v>
+      </c>
+      <c r="G110" s="3">
+        <v>140</v>
+      </c>
+      <c r="H110" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I110" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J110" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A111" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B111" s="6">
+        <v>2171</v>
+      </c>
+      <c r="C111" s="3">
+        <v>72</v>
+      </c>
+      <c r="D111" s="3">
+        <v>37</v>
+      </c>
+      <c r="E111" s="3">
+        <v>204</v>
+      </c>
+      <c r="F111" s="3">
+        <v>2328</v>
+      </c>
+      <c r="G111" s="3">
+        <v>159</v>
+      </c>
+      <c r="H111" s="3">
+        <v>3250</v>
+      </c>
+      <c r="I111" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J111" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating FoodLog files 29/04/2018
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79CD2E6-A5DE-4263-B274-4864BD769BB7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AED1A0-6ED2-4A36-AF9C-3FB2C27A0974}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{2FDD2F76-DCBF-453F-AE6A-59BCC3816064}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Date</t>
   </si>
@@ -385,6 +385,30 @@
   </si>
   <si>
     <t>21-04-2018</t>
+  </si>
+  <si>
+    <t>22-04-2018</t>
+  </si>
+  <si>
+    <t>23-04-2018</t>
+  </si>
+  <si>
+    <t>24-04-2018</t>
+  </si>
+  <si>
+    <t>25-04-2018</t>
+  </si>
+  <si>
+    <t>26-04-2018</t>
+  </si>
+  <si>
+    <t>27-04-2018</t>
+  </si>
+  <si>
+    <t>28-04-2018</t>
+  </si>
+  <si>
+    <t>29-04-2018</t>
   </si>
 </sst>
 </file>
@@ -436,7 +460,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -450,6 +474,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -771,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="L109" sqref="L109"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="L113" sqref="L113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3059,11 +3084,11 @@
         <v>3250</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I111" si="2">IF(H67&gt;=2200,"Yes","No")</f>
+        <f t="shared" ref="I67:I119" si="2">IF(H67&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J111" si="3">IF(B67&lt;=1800,"Yes","No")</f>
+        <f t="shared" ref="J67:J119" si="3">IF(B67&lt;=1800,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4559,6 +4584,278 @@
         <v>Yes</v>
       </c>
       <c r="J111" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A112" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112" s="6">
+        <v>2058</v>
+      </c>
+      <c r="C112" s="3">
+        <v>61</v>
+      </c>
+      <c r="D112" s="3">
+        <v>21</v>
+      </c>
+      <c r="E112" s="3">
+        <v>230</v>
+      </c>
+      <c r="F112" s="3">
+        <v>3285</v>
+      </c>
+      <c r="G112" s="3">
+        <v>147</v>
+      </c>
+      <c r="H112" s="3">
+        <v>3000</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J112" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A113" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113" s="6">
+        <v>1891</v>
+      </c>
+      <c r="C113" s="3">
+        <v>52</v>
+      </c>
+      <c r="D113" s="3">
+        <v>30</v>
+      </c>
+      <c r="E113" s="3">
+        <v>174</v>
+      </c>
+      <c r="F113" s="3">
+        <v>4042</v>
+      </c>
+      <c r="G113" s="3">
+        <v>181</v>
+      </c>
+      <c r="H113" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J113" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A114" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B114" s="6">
+        <v>1658</v>
+      </c>
+      <c r="C114" s="3">
+        <v>46</v>
+      </c>
+      <c r="D114" s="3">
+        <v>16</v>
+      </c>
+      <c r="E114" s="3">
+        <v>145</v>
+      </c>
+      <c r="F114" s="3">
+        <v>2632</v>
+      </c>
+      <c r="G114" s="3">
+        <v>155</v>
+      </c>
+      <c r="H114" s="3">
+        <v>3000</v>
+      </c>
+      <c r="I114" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J114" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A115" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B115" s="6">
+        <v>1571</v>
+      </c>
+      <c r="C115" s="3">
+        <v>45</v>
+      </c>
+      <c r="D115" s="3">
+        <v>11</v>
+      </c>
+      <c r="E115" s="3">
+        <v>126</v>
+      </c>
+      <c r="F115" s="3">
+        <v>3182</v>
+      </c>
+      <c r="G115" s="3">
+        <v>149</v>
+      </c>
+      <c r="H115" s="3">
+        <v>2500</v>
+      </c>
+      <c r="I115" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J115" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A116" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116" s="6">
+        <v>2050</v>
+      </c>
+      <c r="C116" s="3">
+        <v>111</v>
+      </c>
+      <c r="D116" s="3">
+        <v>9</v>
+      </c>
+      <c r="E116" s="3">
+        <v>86</v>
+      </c>
+      <c r="F116" s="3">
+        <v>2649</v>
+      </c>
+      <c r="G116" s="3">
+        <v>166</v>
+      </c>
+      <c r="H116" s="3">
+        <v>3000</v>
+      </c>
+      <c r="I116" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J116" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A117" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B117" s="6">
+        <v>2010</v>
+      </c>
+      <c r="C117" s="3">
+        <v>77</v>
+      </c>
+      <c r="D117" s="3">
+        <v>13</v>
+      </c>
+      <c r="E117" s="3">
+        <v>191</v>
+      </c>
+      <c r="F117" s="3">
+        <v>4375</v>
+      </c>
+      <c r="G117" s="3">
+        <v>128</v>
+      </c>
+      <c r="H117" s="3">
+        <v>1750</v>
+      </c>
+      <c r="I117" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J117" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A118" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B118" s="6">
+        <v>1832</v>
+      </c>
+      <c r="C118" s="3">
+        <v>62</v>
+      </c>
+      <c r="D118" s="3">
+        <v>10</v>
+      </c>
+      <c r="E118" s="3">
+        <v>158</v>
+      </c>
+      <c r="F118" s="3">
+        <v>2212</v>
+      </c>
+      <c r="G118" s="3">
+        <v>133</v>
+      </c>
+      <c r="H118" s="3">
+        <v>1500</v>
+      </c>
+      <c r="I118" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J118" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A119" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B119" s="6">
+        <v>2236</v>
+      </c>
+      <c r="C119" s="3">
+        <v>104</v>
+      </c>
+      <c r="D119" s="3">
+        <v>23</v>
+      </c>
+      <c r="E119" s="3">
+        <v>183</v>
+      </c>
+      <c r="F119" s="3">
+        <v>4231</v>
+      </c>
+      <c r="G119" s="3">
+        <v>148</v>
+      </c>
+      <c r="H119" s="3">
+        <v>3250</v>
+      </c>
+      <c r="I119" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J119" t="str">
         <f t="shared" si="3"/>
         <v>No</v>
       </c>

</xml_diff>

<commit_message>
Updating FoodLog file 06/05/2018
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D58C77-C706-4B3A-8248-B22075FF9A44}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABEA3EB-2E6A-4947-B8A5-11D7436E052E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{2FDD2F76-DCBF-453F-AE6A-59BCC3816064}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -107,13 +107,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -430,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:K119"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2718,11 +2719,11 @@
         <v>3250</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I119" si="2">IF(H67&gt;=2200,"Yes","No")</f>
+        <f t="shared" ref="I67:I126" si="2">IF(H67&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J119" si="3">IF(B67&lt;=1800,"Yes","No")</f>
+        <f t="shared" ref="J67:J126" si="3">IF(B67&lt;=1800,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4492,6 +4493,244 @@
       <c r="J119" t="str">
         <f t="shared" si="3"/>
         <v>No</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A120" s="6">
+        <v>43220</v>
+      </c>
+      <c r="B120" s="2">
+        <v>1884</v>
+      </c>
+      <c r="C120" s="1">
+        <v>57</v>
+      </c>
+      <c r="D120" s="1">
+        <v>27</v>
+      </c>
+      <c r="E120" s="1">
+        <v>162</v>
+      </c>
+      <c r="F120" s="1">
+        <v>3415</v>
+      </c>
+      <c r="G120" s="1">
+        <v>178</v>
+      </c>
+      <c r="H120" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I120" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J120" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A121" s="6">
+        <v>43221</v>
+      </c>
+      <c r="B121" s="2">
+        <v>1679</v>
+      </c>
+      <c r="C121" s="1">
+        <v>54</v>
+      </c>
+      <c r="D121" s="1">
+        <v>25</v>
+      </c>
+      <c r="E121" s="1">
+        <v>151</v>
+      </c>
+      <c r="F121" s="1">
+        <v>2744</v>
+      </c>
+      <c r="G121" s="1">
+        <v>144</v>
+      </c>
+      <c r="H121" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I121" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J121" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A122" s="6">
+        <v>43222</v>
+      </c>
+      <c r="B122" s="2">
+        <v>1706</v>
+      </c>
+      <c r="C122" s="1">
+        <v>66</v>
+      </c>
+      <c r="D122" s="1">
+        <v>16</v>
+      </c>
+      <c r="E122" s="1">
+        <v>176</v>
+      </c>
+      <c r="F122" s="1">
+        <v>2429</v>
+      </c>
+      <c r="G122" s="1">
+        <v>100</v>
+      </c>
+      <c r="H122" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I122" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J122" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A123" s="6">
+        <v>43223</v>
+      </c>
+      <c r="B123" s="2">
+        <v>1227</v>
+      </c>
+      <c r="C123" s="1">
+        <v>38</v>
+      </c>
+      <c r="D123" s="1">
+        <v>19</v>
+      </c>
+      <c r="E123" s="1">
+        <v>132</v>
+      </c>
+      <c r="F123" s="1">
+        <v>2382</v>
+      </c>
+      <c r="G123" s="1">
+        <v>90</v>
+      </c>
+      <c r="H123" s="1">
+        <v>2500</v>
+      </c>
+      <c r="I123" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J123" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A124" s="6">
+        <v>43224</v>
+      </c>
+      <c r="B124" s="2">
+        <v>1370</v>
+      </c>
+      <c r="C124" s="1">
+        <v>43</v>
+      </c>
+      <c r="D124" s="1">
+        <v>15</v>
+      </c>
+      <c r="E124" s="1">
+        <v>167</v>
+      </c>
+      <c r="F124" s="1">
+        <v>2791</v>
+      </c>
+      <c r="G124" s="1">
+        <v>74</v>
+      </c>
+      <c r="H124" s="1">
+        <v>3500</v>
+      </c>
+      <c r="I124" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J124" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A125" s="6">
+        <v>43225</v>
+      </c>
+      <c r="B125" s="2">
+        <v>2274</v>
+      </c>
+      <c r="C125" s="1">
+        <v>63</v>
+      </c>
+      <c r="D125" s="1">
+        <v>41</v>
+      </c>
+      <c r="E125" s="1">
+        <v>257</v>
+      </c>
+      <c r="F125" s="1">
+        <v>3950</v>
+      </c>
+      <c r="G125" s="1">
+        <v>182</v>
+      </c>
+      <c r="H125" s="1">
+        <v>3250</v>
+      </c>
+      <c r="I125" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J125" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A126" s="6">
+        <v>43226</v>
+      </c>
+      <c r="B126" s="2">
+        <v>1637</v>
+      </c>
+      <c r="C126" s="1">
+        <v>49</v>
+      </c>
+      <c r="D126" s="1">
+        <v>24</v>
+      </c>
+      <c r="E126" s="1">
+        <v>174</v>
+      </c>
+      <c r="F126" s="1">
+        <v>1966</v>
+      </c>
+      <c r="G126" s="1">
+        <v>121</v>
+      </c>
+      <c r="H126" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I126" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J126" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating FoodLog file 13/05/2018
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABEA3EB-2E6A-4947-B8A5-11D7436E052E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA2B9D02-A055-418E-9950-734A529D53FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{2FDD2F76-DCBF-453F-AE6A-59BCC3816064}"/>
   </bookViews>
@@ -61,9 +61,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="170" formatCode="0_ ;\-0\ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -107,7 +108,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -115,6 +116,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -431,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:K126"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2719,11 +2721,11 @@
         <v>3250</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I126" si="2">IF(H67&gt;=2200,"Yes","No")</f>
+        <f t="shared" ref="I67:I133" si="2">IF(H67&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J126" si="3">IF(B67&lt;=1800,"Yes","No")</f>
+        <f t="shared" ref="J67:J130" si="3">IF(B67&lt;=1800,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4730,6 +4732,244 @@
       </c>
       <c r="J126" t="str">
         <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A127" s="6">
+        <v>43227</v>
+      </c>
+      <c r="B127" s="7">
+        <v>1522</v>
+      </c>
+      <c r="C127" s="1">
+        <v>43</v>
+      </c>
+      <c r="D127" s="1">
+        <v>20</v>
+      </c>
+      <c r="E127" s="1">
+        <v>143</v>
+      </c>
+      <c r="F127" s="1">
+        <v>2691</v>
+      </c>
+      <c r="G127" s="1">
+        <v>136</v>
+      </c>
+      <c r="H127" s="1">
+        <v>3250</v>
+      </c>
+      <c r="I127" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J127" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A128" s="6">
+        <v>43228</v>
+      </c>
+      <c r="B128" s="7">
+        <v>1568</v>
+      </c>
+      <c r="C128" s="1">
+        <v>42</v>
+      </c>
+      <c r="D128" s="1">
+        <v>30</v>
+      </c>
+      <c r="E128" s="1">
+        <v>166</v>
+      </c>
+      <c r="F128" s="1">
+        <v>2811</v>
+      </c>
+      <c r="G128" s="1">
+        <v>137</v>
+      </c>
+      <c r="H128" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I128" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J128" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A129" s="6">
+        <v>43229</v>
+      </c>
+      <c r="B129" s="7">
+        <v>1539</v>
+      </c>
+      <c r="C129" s="1">
+        <v>64</v>
+      </c>
+      <c r="D129" s="1">
+        <v>17</v>
+      </c>
+      <c r="E129" s="1">
+        <v>131</v>
+      </c>
+      <c r="F129" s="1">
+        <v>2694</v>
+      </c>
+      <c r="G129" s="1">
+        <v>114</v>
+      </c>
+      <c r="H129" s="1">
+        <v>5000</v>
+      </c>
+      <c r="I129" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A130" s="6">
+        <v>43230</v>
+      </c>
+      <c r="B130" s="7">
+        <v>1507</v>
+      </c>
+      <c r="C130" s="1">
+        <v>35</v>
+      </c>
+      <c r="D130" s="1">
+        <v>25</v>
+      </c>
+      <c r="E130" s="1">
+        <v>180</v>
+      </c>
+      <c r="F130" s="1">
+        <v>2938</v>
+      </c>
+      <c r="G130" s="1">
+        <v>118</v>
+      </c>
+      <c r="H130" s="1">
+        <v>4500</v>
+      </c>
+      <c r="I130" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J130" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A131" s="6">
+        <v>43231</v>
+      </c>
+      <c r="B131" s="7">
+        <v>1473</v>
+      </c>
+      <c r="C131" s="1">
+        <v>43</v>
+      </c>
+      <c r="D131" s="1">
+        <v>15</v>
+      </c>
+      <c r="E131" s="1">
+        <v>173</v>
+      </c>
+      <c r="F131" s="1">
+        <v>2805</v>
+      </c>
+      <c r="G131" s="1">
+        <v>75</v>
+      </c>
+      <c r="H131" s="1">
+        <v>6500</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J131" t="str">
+        <f t="shared" ref="J131:J133" si="4">IF(B131&lt;=1800,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A132" s="6">
+        <v>43232</v>
+      </c>
+      <c r="B132" s="7">
+        <v>1806</v>
+      </c>
+      <c r="C132" s="1">
+        <v>88</v>
+      </c>
+      <c r="D132" s="1">
+        <v>16</v>
+      </c>
+      <c r="E132" s="1">
+        <v>142</v>
+      </c>
+      <c r="F132" s="1">
+        <v>3333</v>
+      </c>
+      <c r="G132" s="1">
+        <v>110</v>
+      </c>
+      <c r="H132" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J132" t="str">
+        <f t="shared" si="4"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A133" s="6">
+        <v>43233</v>
+      </c>
+      <c r="B133" s="7">
+        <v>1765</v>
+      </c>
+      <c r="C133" s="1">
+        <v>41</v>
+      </c>
+      <c r="D133" s="1">
+        <v>17</v>
+      </c>
+      <c r="E133" s="1">
+        <v>240</v>
+      </c>
+      <c r="F133" s="1">
+        <v>3214</v>
+      </c>
+      <c r="G133" s="1">
+        <v>97</v>
+      </c>
+      <c r="H133" s="1">
+        <v>1500</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J133" t="str">
+        <f t="shared" si="4"/>
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating FoodLog file 22/05/2018
</commit_message>
<xml_diff>
--- a/datasets/FoodLog.xlsx
+++ b/datasets/FoodLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA2B9D02-A055-418E-9950-734A529D53FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EC108A-A860-4792-8EF6-898ED12BAFDA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{2FDD2F76-DCBF-453F-AE6A-59BCC3816064}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
-    <numFmt numFmtId="170" formatCode="0_ ;\-0\ "/>
+    <numFmt numFmtId="165" formatCode="0_ ;\-0\ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -116,7 +116,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -433,16 +433,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7EEB24-B88B-49C1-86AC-89EA1A5C8C95}">
-  <dimension ref="A1:K133"/>
+  <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+      <selection activeCell="L137" sqref="L137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.7265625" style="1"/>
     <col min="5" max="5" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.453125" style="1" bestFit="1" customWidth="1"/>
@@ -2721,7 +2721,7 @@
         <v>3250</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I133" si="2">IF(H67&gt;=2200,"Yes","No")</f>
+        <f t="shared" ref="I67:I141" si="2">IF(H67&gt;=2200,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="J67" t="str">
@@ -4901,7 +4901,7 @@
         <v>Yes</v>
       </c>
       <c r="J131" t="str">
-        <f t="shared" ref="J131:J133" si="4">IF(B131&lt;=1800,"Yes","No")</f>
+        <f t="shared" ref="J131:J141" si="4">IF(B131&lt;=1800,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4971,6 +4971,278 @@
       <c r="J133" t="str">
         <f t="shared" si="4"/>
         <v>Yes</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A134" s="6">
+        <v>43234</v>
+      </c>
+      <c r="B134" s="3">
+        <v>2041</v>
+      </c>
+      <c r="C134" s="1">
+        <v>67</v>
+      </c>
+      <c r="D134" s="1">
+        <v>31</v>
+      </c>
+      <c r="E134" s="1">
+        <v>169</v>
+      </c>
+      <c r="F134" s="1">
+        <v>3468</v>
+      </c>
+      <c r="G134" s="1">
+        <v>187</v>
+      </c>
+      <c r="H134" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J134" t="str">
+        <f t="shared" si="4"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A135" s="6">
+        <v>43235</v>
+      </c>
+      <c r="B135" s="3">
+        <v>1507</v>
+      </c>
+      <c r="C135" s="1">
+        <v>35</v>
+      </c>
+      <c r="D135" s="1">
+        <v>25</v>
+      </c>
+      <c r="E135" s="1">
+        <v>180</v>
+      </c>
+      <c r="F135" s="1">
+        <v>2938</v>
+      </c>
+      <c r="G135" s="1">
+        <v>118</v>
+      </c>
+      <c r="H135" s="1">
+        <v>3500</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J135" t="str">
+        <f t="shared" si="4"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A136" s="6">
+        <v>43236</v>
+      </c>
+      <c r="B136" s="3">
+        <v>1681</v>
+      </c>
+      <c r="C136" s="1">
+        <v>47</v>
+      </c>
+      <c r="D136" s="1">
+        <v>13</v>
+      </c>
+      <c r="E136" s="1">
+        <v>131</v>
+      </c>
+      <c r="F136" s="1">
+        <v>3242</v>
+      </c>
+      <c r="G136" s="1">
+        <v>169</v>
+      </c>
+      <c r="H136" s="1">
+        <v>3250</v>
+      </c>
+      <c r="I136" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J136" t="str">
+        <f t="shared" si="4"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A137" s="6">
+        <v>43237</v>
+      </c>
+      <c r="B137" s="3">
+        <v>1522</v>
+      </c>
+      <c r="C137" s="1">
+        <v>43</v>
+      </c>
+      <c r="D137" s="1">
+        <v>20</v>
+      </c>
+      <c r="E137" s="1">
+        <v>143</v>
+      </c>
+      <c r="F137" s="1">
+        <v>2691</v>
+      </c>
+      <c r="G137" s="1">
+        <v>136</v>
+      </c>
+      <c r="H137" s="1">
+        <v>3500</v>
+      </c>
+      <c r="I137" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J137" t="str">
+        <f t="shared" si="4"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A138" s="6">
+        <v>43238</v>
+      </c>
+      <c r="B138" s="3">
+        <v>1727</v>
+      </c>
+      <c r="C138" s="1">
+        <v>46</v>
+      </c>
+      <c r="D138" s="1">
+        <v>22</v>
+      </c>
+      <c r="E138" s="1">
+        <v>154</v>
+      </c>
+      <c r="F138" s="1">
+        <v>3362</v>
+      </c>
+      <c r="G138" s="1">
+        <v>170</v>
+      </c>
+      <c r="H138" s="1">
+        <v>3250</v>
+      </c>
+      <c r="I138" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J138" t="str">
+        <f t="shared" si="4"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A139" s="6">
+        <v>43239</v>
+      </c>
+      <c r="B139" s="3">
+        <v>2062</v>
+      </c>
+      <c r="C139" s="1">
+        <v>101</v>
+      </c>
+      <c r="D139" s="1">
+        <v>24</v>
+      </c>
+      <c r="E139" s="1">
+        <v>178</v>
+      </c>
+      <c r="F139" s="1">
+        <v>3590</v>
+      </c>
+      <c r="G139" s="1">
+        <v>117</v>
+      </c>
+      <c r="H139" s="1">
+        <v>1250</v>
+      </c>
+      <c r="I139" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J139" t="str">
+        <f t="shared" si="4"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A140" s="6">
+        <v>43240</v>
+      </c>
+      <c r="B140" s="3">
+        <v>1861</v>
+      </c>
+      <c r="C140" s="1">
+        <v>45</v>
+      </c>
+      <c r="D140" s="1">
+        <v>21</v>
+      </c>
+      <c r="E140" s="1">
+        <v>218</v>
+      </c>
+      <c r="F140" s="1">
+        <v>3873</v>
+      </c>
+      <c r="G140" s="1">
+        <v>139</v>
+      </c>
+      <c r="H140" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I140" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="J140" t="str">
+        <f t="shared" si="4"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A141" s="6">
+        <v>43241</v>
+      </c>
+      <c r="B141" s="3">
+        <v>1884</v>
+      </c>
+      <c r="C141" s="1">
+        <v>57</v>
+      </c>
+      <c r="D141" s="1">
+        <v>27</v>
+      </c>
+      <c r="E141" s="1">
+        <v>162</v>
+      </c>
+      <c r="F141" s="1">
+        <v>3415</v>
+      </c>
+      <c r="G141" s="1">
+        <v>178</v>
+      </c>
+      <c r="H141" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I141" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="J141" t="str">
+        <f t="shared" si="4"/>
+        <v>No</v>
       </c>
     </row>
   </sheetData>

</xml_diff>